<commit_message>
update Rag prompt and add document
</commit_message>
<xml_diff>
--- a/MEC-question-V0.2.xlsx
+++ b/MEC-question-V0.2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">عنوان</t>
   </si>
@@ -578,16 +578,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">در سامانه فرابانک صرفاً به صورت غیرحضوری و با استفاده از برنامه کاربردی امضای ملت امکان‌پذیر است. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Noto Sans Devanagari"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> نرخ سود وام بهان ۲۳ درصد است.</t>
+      <t xml:space="preserve">در سامانه فرابانک صرفاً به صورت غیرحضوری و با استفاده از برنامه کاربردی امضای ملت امکان‌پذیر است.  نرخ سود وام بهان ۲۳ درصد است.</t>
     </r>
   </si>
   <si>
@@ -840,18 +831,9 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">نرخ سود وام فرابانک ۲۳ درصد است.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Noto Sans Devanagari"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">نرخ سود وام فرابانک ۲۳ درصد است. </t>
     </r>
   </si>
   <si>
@@ -947,7 +929,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ماه می‌باشد.
-در انواع عقد مرابحه، عقد جعاله و کارت اعتباری اعطا می‌شود. سقف وام مبلغ ۳۰۰ میلیون تومان است و رتبه‌های مجاز برای دریافت وام </t>
+در انواع عقد مرابحه، عقد جعاله و کارت اعتباری اعطا می‌شود. سقف وام مبلغ ۳۰۰ میلیون تومان است و رتبه‌های اعتباری مجاز برای دریافت وام </t>
     </r>
     <r>
       <rPr>
@@ -1055,6 +1037,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">نرخ سود وام شایان، ۱۴، ۱۸ و ۲۳ درصد است.</t>
     </r>
@@ -1211,7 +1194,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">سقف وام مبلغ ۳۰۰ میلیون تومان است و رتبه‌های مجاز برای دریافت وام </t>
+      <t xml:space="preserve">سقف وام مبلغ ۳۰۰ میلیون تومان است و رتبه‌های اعتباری مجاز برای دریافت وام </t>
     </r>
     <r>
       <rPr>
@@ -1371,16 +1354,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">تا مبلغ صد میلیون تومان یک ضامن و بالاتر از این مبلغ دو ضامن الزامی است. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Noto Sans Devanagari"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">نرخ سود وام نیک وام ۴ درصد است.</t>
+      <t xml:space="preserve">تا مبلغ صد میلیون تومان یک ضامن و بالاتر از این مبلغ دو ضامن الزامی است. نرخ سود وام نیک وام ۴ درصد است.</t>
     </r>
   </si>
   <si>
@@ -1430,7 +1404,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">رتبه‌های مجاز برای دریافت وام </t>
+      <t xml:space="preserve">رتبه‌های اعتباری مجاز برای دریافت وام </t>
     </r>
     <r>
       <rPr>
@@ -1815,6 +1789,285 @@
       <t xml:space="preserve">A, B, C, D  و  E بیان می شود.
 </t>
     </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">همچنین </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">رتبه‌های اعتباری مجاز برای دریافت وام شایان </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">E </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">،</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">D </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">،</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">C </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">،</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">،</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">A است .
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">رتبه‌های اعتباری مجاز برای دریافت وام نیک وام </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">C </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">،</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">،</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">است</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">رتبه های اعتباری مجاز برای دریافت وام بهان </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">A, B است.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">رتبه‌های اعتباری مجاز برای دریافت وام فرابانک </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">C </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">،</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">،</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">است</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">معدل حساب</t>
@@ -1867,6 +2120,51 @@
   <si>
     <t xml:space="preserve">توان بازپرداخت (قدرت بازپرداخت) به توانایی یک فرد در بازپرداخت بدهی‌ها و تعهدات مالی خود در موعد مقرر اشاره دارد. این مفهوم در ارزیابی اعتباری و تصمیم گیری‌های مالی بسیار مهم است، زیرا نشان دهنده میزان ریسک مرتبط با اعطای وام یا تسهیلات به شخص مورد نظر است. نحوه محاسبه توان‌بازپرداخت:   ۶۰ درصد درآمد - (قسط‌های در جریان وام‌گیرنده + قسط‌های ضمانت شده توسط وام‌گیرنده)
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> مهان</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">مهان یک نوع مشتری خاص است که در بانک ملت تعریف شده است</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">چنانچه در شمار مشتریان مهان بانک ملت قرار گرفته باشید، می‌توانید از خدمات و امکانات ویژه‌ای که بانک برای این دسته از مشتریان خود درنظر گرفته است استفاده نمایید</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1877,7 +2175,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1919,6 +2217,12 @@
       <color theme="1"/>
       <name val="Noto Sans Devanagari"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="B Homa"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2223,8 +2527,8 @@
   </sheetPr>
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2353,7 +2657,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="90.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="105.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
@@ -2361,7 +2665,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="76.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
@@ -2377,7 +2681,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="60.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="60.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
@@ -2409,7 +2713,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="209.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="200.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>44</v>
       </c>
@@ -2434,8 +2738,12 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
+      <c r="A26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="8"/>

</xml_diff>